<commit_message>
minor changes to jhol.java and configuration
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DataSheet.xlsx
+++ b/src/test/resources/Data/DataSheet.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2B022A-8E42-44CD-AD7D-C10E8486BD22}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="6375" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterSheet" sheetId="1" r:id="rId1"/>
@@ -13,7 +14,7 @@
     <sheet name="Dropdowns" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Google!$A$2:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Google!$A$2:$G$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
-  <si>
-    <t>LOB</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Yes</t>
   </si>
@@ -132,37 +130,43 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Jhol (film) - Wikipedia</t>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Firefox</t>
+  </si>
+  <si>
+    <t>Safari</t>
+  </si>
+  <si>
+    <t>windows</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Another Jhol</t>
+  </si>
+  <si>
+    <t>Videos</t>
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Jhol_(film)</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>IE</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Firefox</t>
-  </si>
-  <si>
-    <t>Safari</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>windows</t>
+    <t>Sheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -279,7 +283,47 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -575,11 +619,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,41 +633,41 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" location="Google!A1" display="Google"/>
+    <hyperlink ref="A2" location="Google!A1" display="Google" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Dropdowns!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Dropdowns!$C$2:$C$5</xm:f>
           </x14:formula1>
@@ -636,14 +680,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,34 +708,34 @@
       <c r="C1" s="8"/>
       <c r="D1" s="6"/>
       <c r="E1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="G2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -699,35 +743,85 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>32</v>
+      <c r="G4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E3"/>
+  <autoFilter ref="A2:G2" xr:uid="{0FAA4B87-CC90-4D04-97F8-3E01A0E69397}"/>
   <mergeCells count="1">
     <mergeCell ref="E1:F1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" operator="containsText" text="fail">
+  <conditionalFormatting sqref="D1:D3 D6:D1048576">
+    <cfRule type="containsText" dxfId="5" priority="7" stopIfTrue="1" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",D1)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" stopIfTrue="1" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="containsText" dxfId="3" priority="3" stopIfTrue="1" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",D4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" stopIfTrue="1" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",D4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",D5)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" stopIfTrue="1" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH("pass",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("pass",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -735,17 +829,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Dropdowns!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Dropdowns!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:C1048576</xm:sqref>
+          <xm:sqref>C6:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -754,7 +848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -772,7 +866,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
@@ -781,7 +875,7 @@
       <c r="J1" s="11"/>
       <c r="K1" s="3"/>
       <c r="L1" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
@@ -793,61 +887,61 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -861,7 +955,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -875,42 +969,42 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes to reportermanager and jhol
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DataSheet.xlsx
+++ b/src/test/resources/Data/DataSheet.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
   <si>
     <t>Yes</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Sheet</t>
+  </si>
+  <si>
+    <t>https://timesofindia.indiatimes.com/entertainment/bengali/movie-reviews/macher-jhol/movie-review/60174378.cms</t>
   </si>
 </sst>
 </file>
@@ -788,9 +791,15 @@
       <c r="C5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="G5" s="6" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
BringToFront added for windows automation
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DataSheet.xlsx
+++ b/src/test/resources/Data/DataSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>Yes</t>
   </si>
@@ -102,9 +102,6 @@
     <t>TestCaseDescription</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>Optional</t>
   </si>
   <si>
@@ -159,37 +156,31 @@
     <t>Sheet</t>
   </si>
   <si>
-    <t>http://www.jamuura.com/blog/life-is-all-about-contrast-abhishek-verma-on-his-upcoming-short-animation-maacher-jhol/</t>
-  </si>
-  <si>
-    <t>WDPR - Walt Disney Parks and Resorts | AcronymFinder</t>
-  </si>
-  <si>
-    <t>https://www.acronymfinder.com/Walt-Disney-Parks-and-Resorts-(WDPR).html</t>
-  </si>
-  <si>
-    <t>Unscramble AWIJP Words With AWIJP Unscrambled</t>
-  </si>
-  <si>
-    <t>http://www.unscramblerer.com/unscramble-word/awijp</t>
-  </si>
-  <si>
     <t>Macher Jhol Movie Review {3.5/5}: Critic Review of Macher Jhol by ...</t>
   </si>
   <si>
     <t>https://timesofindia.indiatimes.com/entertainment/bengali/movie-reviews/macher-jhol/movie-review/60174378.cms</t>
   </si>
   <si>
-    <t>What is a Construction Phase Health and Safety Plan? | Simply-Docs</t>
-  </si>
-  <si>
-    <t>https://simply-docs.co.uk/Construction-Design--Management-Regulations-2015/What-is-a-Construction-Phase-Health-and-Safety-Plan</t>
-  </si>
-  <si>
-    <t>Images for yApATb</t>
-  </si>
-  <si>
-    <t>https://sanskritdocuments.org/marathi/documents/vasanta.ps</t>
+    <t>Adidas One Grey W Gum4 Campus Core Black Footshop XgrXIq</t>
+  </si>
+  <si>
+    <t>http://helper.extrapulpe.com/hcap-3-spanish.mdoc</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>windows</t>
   </si>
 </sst>
 </file>
@@ -234,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -257,38 +248,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -298,13 +263,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -662,24 +624,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -710,13 +672,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,12 +698,12 @@
       <c r="B1" s="6"/>
       <c r="C1" s="8"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="9" t="s">
-        <v>28</v>
+      <c r="E1" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -758,81 +720,98 @@
         <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="G2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="G4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="C6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:G2"/>
@@ -904,25 +883,25 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1011,10 +990,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1022,7 +1001,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1033,17 +1012,17 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arguments introduced for filter
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DataSheet.xlsx
+++ b/src/test/resources/Data/DataSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="56">
   <si>
     <t>Yes</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>fail</t>
+  </si>
+  <si>
+    <t>Zsinj | Wookieepedia | FANDOM powered by Wikia</t>
+  </si>
+  <si>
+    <t>https://starwars.fandom.com/wiki/Zsinj</t>
   </si>
 </sst>
 </file>
@@ -754,13 +760,13 @@
         <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>

</xml_diff>

<commit_message>
autoIt and trace log
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DataSheet.xlsx
+++ b/src/test/resources/Data/DataSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="73">
   <si>
     <t>Yes</t>
   </si>
@@ -193,6 +193,57 @@
   </si>
   <si>
     <t>https://starwars.fandom.com/wiki/Zsinj</t>
+  </si>
+  <si>
+    <t>Grga - Wikipedia</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Grga</t>
+  </si>
+  <si>
+    <t>Evergy, Inc. (EVRG) Stock Price, Quote, History &amp; News - Yahoo Finance</t>
+  </si>
+  <si>
+    <t>https://finance.yahoo.com/q?s=EVRG</t>
+  </si>
+  <si>
+    <t>Images for Ogdqf</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=oGdqf-ruCR8</t>
+  </si>
+  <si>
+    <t>Fs MTZmanus - Home | Facebook</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/Fs-MTZmanus-348567662008350/</t>
+  </si>
+  <si>
+    <t>Images for pqRHQF</t>
+  </si>
+  <si>
+    <t>http://www.themegatons.fr/ooxrtn/murderer/fyzfz-6.htm</t>
+  </si>
+  <si>
+    <t>Erikkc (@xiaopg) • Instagram photos and videos</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/xiaopg/?hl=en</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Dharmesh Sir CRAZY Dance With Shakti, Raghav &amp; Punit At Dance ...</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=jnDdnL_ZPiI</t>
+  </si>
+  <si>
+    <t>#rwif hashtag on Instagram • Photos and Videos</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/explore/tags/rwif/?hl=en</t>
   </si>
 </sst>
 </file>
@@ -763,10 +814,10 @@
         <v>53</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -832,7 +883,7 @@
         <v>51</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>

</xml_diff>